<commit_message>
added condition if marketDays manual
</commit_message>
<xml_diff>
--- a/_userInput.xlsx
+++ b/_userInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gdrive Kevin\Gabi, SArs, MBA\pySpillovers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B57F37-0828-4B27-B747-45E12E8BC6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363FAEF0-D04F-407E-9A90-15AFD9A87084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36768" yWindow="4788" windowWidth="17280" windowHeight="8976" xr2:uid="{21F63A62-AB76-45F4-89AA-BDEC09217443}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Volatility Diebold</t>
   </si>
   <si>
-    <t>Auto</t>
-  </si>
-  <si>
     <t>VALUE</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>manualMarketDays</t>
+  </si>
+  <si>
+    <t>Manual</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,12 +530,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4">
         <v>43466</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4">
         <v>44196</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>1</v>
@@ -559,23 +559,23 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="7">
-        <v>365</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="8">
         <f ca="1">YEAR(TODAY())</f>
@@ -584,7 +584,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
         <v>247</v>

</xml_diff>

<commit_message>
done calcSpilloversTable, and adjust functions so people can reuse it
</commit_message>
<xml_diff>
--- a/_userInput.xlsx
+++ b/_userInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gdrive Kevin\Gabi, SArs, MBA\pySpillovers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363FAEF0-D04F-407E-9A90-15AFD9A87084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407FF3F9-F2D1-46E1-A555-FD5E6FAD02C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36768" yWindow="4788" windowWidth="17280" windowHeight="8976" xr2:uid="{21F63A62-AB76-45F4-89AA-BDEC09217443}"/>
   </bookViews>
@@ -42,6 +42,9 @@
     <t>Volatility Diebold</t>
   </si>
   <si>
+    <t>Auto</t>
+  </si>
+  <si>
     <t>VALUE</t>
   </si>
   <si>
@@ -64,9 +67,6 @@
   </si>
   <si>
     <t>manualMarketDays</t>
-  </si>
-  <si>
-    <t>Manual</t>
   </si>
 </sst>
 </file>
@@ -530,12 +530,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>43466</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4">
         <v>44196</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>1</v>
@@ -559,15 +559,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="7">
         <v>250</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="8">
         <f ca="1">YEAR(TODAY())</f>
@@ -584,7 +584,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3">
         <v>247</v>

</xml_diff>

<commit_message>
done sensitivity, go to output table and graph
</commit_message>
<xml_diff>
--- a/_userInput.xlsx
+++ b/_userInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gdrive Kevin\Gabi, SArs, MBA\pySpillovers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407FF3F9-F2D1-46E1-A555-FD5E6FAD02C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF26959-AEAF-46A2-8A8D-22F191F730D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36768" yWindow="4788" windowWidth="17280" windowHeight="8976" xr2:uid="{21F63A62-AB76-45F4-89AA-BDEC09217443}"/>
+    <workbookView xWindow="31452" yWindow="2256" windowWidth="17280" windowHeight="8976" xr2:uid="{21F63A62-AB76-45F4-89AA-BDEC09217443}"/>
   </bookViews>
   <sheets>
     <sheet name="userInput" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>SETTINGS</t>
   </si>
@@ -67,6 +67,45 @@
   </si>
   <si>
     <t>manualMarketDays</t>
+  </si>
+  <si>
+    <t>rollingWindow</t>
+  </si>
+  <si>
+    <t>lag_order</t>
+  </si>
+  <si>
+    <t>forecast_horizon</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>NumberFormat: Date</t>
+  </si>
+  <si>
+    <t>Diebold 100, Aslam ASINH</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Auto:market days will be counted based on data for each year, except for end year data using marketDaysYearEnd;Manual: all years using manualMarketDays</t>
+  </si>
+  <si>
+    <t>Fill if using Manual</t>
+  </si>
+  <si>
+    <t>Fill the probable market days for end year data / current year data</t>
+  </si>
+  <si>
+    <t>Auto:decided by system using AIC;&lt;integer&gt;:fill if you know what the lag_order you want to use, example: 4</t>
+  </si>
+  <si>
+    <t>Auto:default 10;&lt;integer&gt;:fill if you know what the forecast_horizon you want to use, example: 10</t>
+  </si>
+  <si>
+    <t>Auto:default 200;&lt;integer&gt;:fill if you know what the rolling_window you want to use, example: 200</t>
   </si>
 </sst>
 </file>
@@ -513,10 +552,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EBA632-F393-47FF-AFDE-AA6DC3438528}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,55 +564,73 @@
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>43466</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4">
-        <v>44196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>44195</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="7">
         <v>250</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -581,13 +638,52 @@
         <f ca="1">YEAR(TODAY())</f>
         <v>2021</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3">
         <v>247</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>